<commit_message>
presentacion semana 4 y los stand up
</commit_message>
<xml_diff>
--- a/Semana 7 - 11  septiembre/Stand_Up_Meeitng_Week_3.xlsx
+++ b/Semana 7 - 11  septiembre/Stand_Up_Meeitng_Week_3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\Documents\GitHub\Ingenieria_Software\Semana 7 - 11  septiembre\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mythe\Documents\GitHub\Ingenieria_Software\Semana 7 - 11  septiembre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189265B5-0A4F-4FFD-957E-ADAB9044A6D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D52C807-9DE2-40F6-BDCC-D477C20541B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3320EE79-9243-42E8-8E5F-EF80DE6A9110}"/>
+    <workbookView xWindow="0" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{3320EE79-9243-42E8-8E5F-EF80DE6A9110}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="35">
   <si>
     <t xml:space="preserve"> MIEMBRO</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>Asistir a reunión de asignación de tareas y realizar nuevos diseños</t>
+  </si>
+  <si>
+    <t>Leer de las diapositivas del profe</t>
+  </si>
+  <si>
+    <t>Asistir a la reunión para el diagrama de requisitos y ayudar con el diagrama de casos de uso</t>
   </si>
 </sst>
 </file>
@@ -464,7 +470,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -762,29 +768,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E4E8726-24EF-4B21-B937-D55FA5E6EA95}">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
-    <col min="3" max="3" width="64.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.21875" customWidth="1"/>
-    <col min="8" max="8" width="13.77734375" customWidth="1"/>
-    <col min="9" max="9" width="13.21875" customWidth="1"/>
-    <col min="10" max="10" width="10.77734375" customWidth="1"/>
-    <col min="11" max="11" width="4.6640625" customWidth="1"/>
-    <col min="12" max="12" width="9.21875" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="64.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="4.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" customWidth="1"/>
     <col min="13" max="13" width="11" customWidth="1"/>
-    <col min="14" max="14" width="10.21875" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>15</v>
       </c>
@@ -802,7 +808,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -818,7 +824,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
@@ -841,7 +847,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>10</v>
       </c>
@@ -854,7 +860,7 @@
       <c r="F4" s="5"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="17"/>
       <c r="B5" s="12" t="s">
         <v>8</v>
@@ -865,7 +871,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="3" t="s">
         <v>9</v>
@@ -876,42 +882,72 @@
       <c r="F6" s="7"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
       <c r="B8" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>12</v>
       </c>
@@ -934,7 +970,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
       <c r="B11" s="12" t="s">
         <v>8</v>
@@ -955,7 +991,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="3" t="s">
         <v>9</v>
@@ -976,7 +1012,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>13</v>
       </c>
@@ -997,7 +1033,7 @@
       </c>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="12" t="s">
         <v>8</v>
@@ -1016,7 +1052,7 @@
       </c>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="3" t="s">
         <v>9</v>
@@ -1035,7 +1071,7 @@
       </c>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>14</v>
       </c>
@@ -1058,7 +1094,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="12" t="s">
         <v>8</v>
@@ -1079,7 +1115,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="4" t="s">
         <v>9</v>

</xml_diff>